<commit_message>
Local database integration via Django models (#17)
* basic model structure

* set time zone to CET

* models prototype

* populate models OK

* update notes w/ migrations

* purge instances before populating

* Delete script_updatefederation.py

* select query by category

* async search for models

* update model database

* async global search via models

* remove old classes
</commit_message>
<xml_diff>
--- a/django/bartocgraphql/fixtures/skosmosinstances.xlsx
+++ b/django/bartocgraphql/fixtures/skosmosinstances.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\itsc-pg2.storage.p.unibas.ch\ub-home$\hinder0000\Documents\GitHub\bartoc-graphql\django\bql\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\itsc-pg2.storage.p.unibas.ch\ub-home$\hinder0000\Documents\GitHub\bartocgraphql\django\bartocgraphql\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +520,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Better query parsing (#47)
* add invalid string exception

* prepare sparql query

* Delete basic.html

* Update index.html

* add context

* fix wildcard parsing

* Update help_text
</commit_message>
<xml_diff>
--- a/django/bartocgraphql/fixtures/skosmosinstances.xlsx
+++ b/django/bartocgraphql/fixtures/skosmosinstances.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>too slow</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>wildcard</t>
   </si>
 </sst>
 </file>
@@ -420,22 +426,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,10 +449,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -456,8 +465,11 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -467,8 +479,11 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -478,8 +493,11 @@
       <c r="C4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -489,19 +507,25 @@
       <c r="C5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -511,8 +535,11 @@
       <c r="C7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -522,11 +549,14 @@
       <c r="C8" s="2">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -536,8 +566,11 @@
       <c r="C9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -545,9 +578,12 @@
         <v>19</v>
       </c>
       <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>